<commit_message>
Update of structures and first product req.
Update
</commit_message>
<xml_diff>
--- a/02_ReqMgn/FMPS_AutoTraderApplication_Customer_Specification.xlsx
+++ b/02_ReqMgn/FMPS_AutoTraderApplication_Customer_Specification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worksite-my.sharepoint.com/personal/bozekpat_schaeffler_com/Documents/Persönlich/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozekpat\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="8_{A3AB8EE7-14D5-4B60-8503-8FD1D30FA8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B20F3EAF-2440-4545-B913-205BB1F4C0A4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44B27A8-0D24-4B4C-9D63-F156EE5D6970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CDDBDED4-4DFE-4FEE-B345-BB3B0A32B25A}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="KPI" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$J$508</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$K$543</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
   <si>
     <t>Requirement Type</t>
   </si>
@@ -116,19 +138,6 @@
   </si>
   <si>
     <t>The product is an application that provides virtual traders. The virtual traders can use trading applications such as Binance, Bitget to carry out automated and autonomous trading of shares, derivatives, crypto, etc. over a period of 24/7 without human intervention. For this purpose, the virtual traders use basic principles, expert and their own practical experience in the field of “technical analysis”.</t>
-  </si>
-  <si>
-    <t>The product shall be available on the following devices:
-- Notebook
-- Tablet
-- Smartphone
-- Smartwatch</t>
-  </si>
-  <si>
-    <t>The product shall be able to interact with the following third party products:
-- Binance
-- Bitget
-- TradingView</t>
   </si>
   <si>
     <t>The product shall be availabe 24/7</t>
@@ -178,15 +187,6 @@
     <t>General</t>
   </si>
   <si>
-    <t>Product Description</t>
-  </si>
-  <si>
-    <t>Product Architecture</t>
-  </si>
-  <si>
-    <t>Product User Interface</t>
-  </si>
-  <si>
     <t>Interface</t>
   </si>
   <si>
@@ -196,24 +196,243 @@
     <t>ATP_ProdSpec</t>
   </si>
   <si>
-    <t>Appendices and References</t>
-  </si>
-  <si>
-    <t>Product and Customer Functions</t>
-  </si>
-  <si>
     <t>Product Release</t>
   </si>
   <si>
     <t>Applicable documents</t>
+  </si>
+  <si>
+    <t>Definition of terms</t>
+  </si>
+  <si>
+    <t>Abbreviations</t>
+  </si>
+  <si>
+    <t>Product architecture</t>
+  </si>
+  <si>
+    <t>Product and customer functions</t>
+  </si>
+  <si>
+    <t>Product user interface</t>
+  </si>
+  <si>
+    <t>Appendices and references</t>
+  </si>
+  <si>
+    <t>Product purpose and description</t>
+  </si>
+  <si>
+    <t>Core Application</t>
+  </si>
+  <si>
+    <t>UI Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The purpose of the product is to partially or fully automate the manual trading of bonds, stocks, forex, crypto, etc. Here, the product is intended to support the effective and efficient use of trading time, as well as to minimize the use of personal lifetime for trading and to maximize the personal monetary profit. The goal is to be achieved by AI traders who trade automatically on accessible exchanges based on technical analysis, the experience of experts and their own experience, and use their information, such as charts and indicators. To achieve this, the user should be able to configure any number of configurable AI traders (e.g. which stock exchange should be used, which risk profile, how much budget, which trading strategies, etc.), which are based on trading profiles provided by the user (third-party povider). The performance and risk classification of the product and the product updates are evaluated, proven and improved via demo accounts.     </t>
+  </si>
+  <si>
+    <t>Stock Exchange Application (third-party provider)</t>
+  </si>
+  <si>
+    <t>Market Information Application (third-party provider)</t>
+  </si>
+  <si>
+    <t>The UI Application shall connect the User with the Core Application</t>
+  </si>
+  <si>
+    <t>The UI Application shall be available on all computer-like devices (e.g. personal computer, notebook, tablet, smartphone, smartwatch)</t>
+  </si>
+  <si>
+    <t>The UI Application shall be the command center to create, re-configure and observe the AI trader by the user, as well as providing a real-time overview of the status and trading success of the AI trader</t>
+  </si>
+  <si>
+    <t>The UI Application shall allow the user to select the exchange they wish to use for trading and to configure their existing account for the exchange</t>
+  </si>
+  <si>
+    <t>The Core Application shall connect User Interface, Trading Knowledge Database and Third-Party Products (e.g. Exchange, Information)</t>
+  </si>
+  <si>
+    <t>Trading Knowledge Database</t>
+  </si>
+  <si>
+    <t>The Core Application shall provide the access and training of trading knowlede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Core Application shall provide the trading algorithm </t>
+  </si>
+  <si>
+    <t>The Core Application shall provide a power lifecycle strategy</t>
+  </si>
+  <si>
+    <t>The Core Application shall provide a error and healing strategy</t>
+  </si>
+  <si>
+    <t>The Core Application shall provide connectors to the computer-like devices</t>
+  </si>
+  <si>
+    <t>The Core Application shall be available 24/7 from the computer-like devices</t>
+  </si>
+  <si>
+    <t>The Core Application shall provide connectors to the stock exchanges</t>
+  </si>
+  <si>
+    <t>The Core Application shall provide connectors to the market information applications</t>
+  </si>
+  <si>
+    <t>The Core Application shall provide the secure access between the connectors and the core application</t>
+  </si>
+  <si>
+    <t>The Trading Knowledge Database shall provide the trading experience to the Core Application</t>
+  </si>
+  <si>
+    <t>The trading experience shall be used by the AI traders</t>
+  </si>
+  <si>
+    <t>The Stock Exchange Application shall connect the Core Application and the Stock Exchange</t>
+  </si>
+  <si>
+    <t>The Stock Exchange Application shall provide a user account for trading</t>
+  </si>
+  <si>
+    <t>The Stock Exchange Application shall provide stock exchange information</t>
+  </si>
+  <si>
+    <t>The Stock Exchange Application shall provide stock market news and indicators</t>
+  </si>
+  <si>
+    <t>The Market Information Application shall connect the Core Application with current real-time information that could potentially have an impact on the exchange</t>
+  </si>
+  <si>
+    <t>The Market Information Application shall connect the Core Application with real-time Market Information</t>
+  </si>
+  <si>
+    <t>The Market Information Application shall provide the Core Application with training material from experts that can be used to build and further develop a trading knowledge database</t>
+  </si>
+  <si>
+    <t>The relevant trading classes of the product
+- Bonds
+- CFDs
+- Cryptos
+- ETFs
+- NFTs
+- Private Equity
+- Raw Materials
+- Stocks</t>
+  </si>
+  <si>
+    <t>Product Logging</t>
+  </si>
+  <si>
+    <t>Initialisierung</t>
+  </si>
+  <si>
+    <t>Hauptbildschirm</t>
+  </si>
+  <si>
+    <t>Konfigurationsbildschirm</t>
+  </si>
+  <si>
+    <t>Historische Datenbildschirm</t>
+  </si>
+  <si>
+    <t>The relevant devices of the product
+- personal computer
+- notebook
+- tablet
+- smartphone
+- smartwatch</t>
+  </si>
+  <si>
+    <t>Product Authentication</t>
+  </si>
+  <si>
+    <t>Product Configuation</t>
+  </si>
+  <si>
+    <t>The product configuration customer function deals with the use cases of configuring the product itself, the third-party tools used and the interface of the third-party tool.</t>
+  </si>
+  <si>
+    <t>The product authentication customer function deals with the use cases of secure login to the product and the third-party tools.</t>
+  </si>
+  <si>
+    <t>Product Status</t>
+  </si>
+  <si>
+    <t>The product status customer function deals with the use cases to determine the status of the product and the third-party tools and to make it visually available to the consumer.</t>
+  </si>
+  <si>
+    <t>The customer function AI Trading deals with the use cases of automated and autonomous trading, as well as manual override.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI Trading </t>
+  </si>
+  <si>
+    <t>AI Trader Training</t>
+  </si>
+  <si>
+    <t>The customer function AI Trader Training deals with the use cases of creating and further developing the trading knowledge database.</t>
+  </si>
+  <si>
+    <t>The customer function product history recording deals with the use cases of recording and logging consumer and trading activities.</t>
+  </si>
+  <si>
+    <t>The customer must log in to the product again when the device ends its power lifecycle or the product is closed by an exit command.</t>
+  </si>
+  <si>
+    <t>When the customer starts the product on their device, a user name and password must be requested for login.</t>
+  </si>
+  <si>
+    <t>The customer function AI Trading must allow the customer to create multiple instances of AI Traders, which trade different trading classes or different products in the same trading class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When creating an AI Trader, the customer must enter and confirm the following parameters for configuring the AI Trader:
+- Exchange
+- Asset
+- Virtual / Real money
+- What is the maximum amount of money to stake from account
+- Maximum risk / leverage level
+- Maximum trading duration
+- Minimum return / profit to be achieved </t>
+  </si>
+  <si>
+    <t>Product Releases</t>
+  </si>
+  <si>
+    <t>Release 1.0.0</t>
+  </si>
+  <si>
+    <t>Release 1.1.0</t>
+  </si>
+  <si>
+    <t>Review Comments</t>
+  </si>
+  <si>
+    <t>The customer function AI Trading must be made available by the product if the product is in the READY state.</t>
+  </si>
+  <si>
+    <t>The creation of an AI Trader must be prevented by the product if:
+- No money is available
+- If there is not enough money to buy a commodity (risk / leverage level taken into account)</t>
+  </si>
+  <si>
+    <t>02_ReqMgn/CommonDefinitionOfTermsAndAbbreviations.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -241,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,11 +468,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -295,23 +529,88 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7FC8FE6-F46E-481C-91D0-30AF018321D6}" name="Tabelle1" displayName="Tabelle1" ref="A1:J34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:J34" xr:uid="{A7FC8FE6-F46E-481C-91D0-30AF018321D6}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{46CA0ADE-60C3-4B69-810F-12D04EC8FDC1}" name="Requirement ID" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7FC8FE6-F46E-481C-91D0-30AF018321D6}" name="Tabelle1" displayName="Tabelle1" ref="A1:K69" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:K69" xr:uid="{A7FC8FE6-F46E-481C-91D0-30AF018321D6}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{46CA0ADE-60C3-4B69-810F-12D04EC8FDC1}" name="Requirement ID" dataDxfId="7">
       <calculatedColumnFormula>IF(B2="","",CONCATENATE(Configuration!$A$2,"_",ROW(B2)-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{3996E0A8-8ED4-47DE-9F71-D002D1E2A479}" name="Requirement Type" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{4DB6534A-98D5-4F9F-AA6F-04DE89817617}" name="Requirement Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5824AFDD-5B18-45C8-9AC1-9D4414C722FE}" name="Requirements Status" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3996E0A8-8ED4-47DE-9F71-D002D1E2A479}" name="Requirement Type" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{4DB6534A-98D5-4F9F-AA6F-04DE89817617}" name="Requirement Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5824AFDD-5B18-45C8-9AC1-9D4414C722FE}" name="Requirements Status" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{182988B6-D010-40C1-9A94-57942788FFA7}" name="Review Comments" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{F046E005-4233-4753-B262-BE2164598DD8}" name="Product Release"/>
-    <tableColumn id="6" xr3:uid="{423296BB-A421-4C7A-B196-CAC33435BD56}" name="Test Case ID" dataDxfId="2">
-      <calculatedColumnFormula>IF(OR(G2="No",G2=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B2)-1))</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{423296BB-A421-4C7A-B196-CAC33435BD56}" name="Test Case ID" dataDxfId="3">
+      <calculatedColumnFormula>IF(OR(H2="No",H2=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B2)-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{68F6AC24-540D-48CB-B1A6-00416E3A8EEE}" name="Test Type" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{68F6AC24-540D-48CB-B1A6-00416E3A8EEE}" name="Test Type" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{B0A9900A-12EE-4E2D-955B-7742260E594C}" name="Test Case Description"/>
-    <tableColumn id="9" xr3:uid="{57BB3F8F-8085-4D6F-BEB4-FA4A1C974F43}" name="Test Case Status" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{57BB3F8F-8085-4D6F-BEB4-FA4A1C974F43}" name="Test Case Status" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{309114D3-8CFC-4381-8B89-807C17100E51}" name="Linked Requirements"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -635,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73031C47-45A9-4ED8-916F-7BC7DB23EFEB}">
-  <dimension ref="A1:J508"/>
+  <dimension ref="A1:K543"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,15 +946,16 @@
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="175.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -669,179 +969,179 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="str">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="str">
         <f>IF(B2="","",CONCATENATE(Configuration!$A$2,"_",ROW(B2)-1))</f>
         <v>ATP_ProdSpec_1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="str">
-        <f>IF(OR(G2="No",G2=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B2)-1))</f>
-        <v/>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="str">
+        <f>IF(OR(H2="No",H2=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B2)-1))</f>
+        <v/>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(B3="","",CONCATENATE(Configuration!$A$2,"_",ROW(B3)-1))</f>
         <v>ATP_ProdSpec_2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="str">
-        <f>IF(OR(G3="No",G3=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B3)-1))</f>
-        <v/>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="1" t="str">
+        <f>IF(OR(H3="No",H3=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B3)-1))</f>
+        <v/>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(B4="","",CONCATENATE(Configuration!$A$2,"_",ROW(B4)-1))</f>
         <v>ATP_ProdSpec_3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="str">
-        <f>IF(OR(G4="No",G4=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B4)-1))</f>
-        <v/>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="1" t="str">
+        <f>IF(OR(H4="No",H4=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B4)-1))</f>
+        <v/>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(B5="","",CONCATENATE(Configuration!$A$2,"_",ROW(B5)-1))</f>
         <v>ATP_ProdSpec_4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="str">
-        <f>IF(OR(G5="No",G5=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B5)-1))</f>
-        <v/>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="1" t="str">
+        <f>IF(OR(H5="No",H5=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B5)-1))</f>
+        <v/>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f>IF(B6="","",CONCATENATE(Configuration!$A$2,"_",ROW(B6)-1))</f>
         <v>ATP_ProdSpec_5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1" t="str">
-        <f>IF(OR(G6="No",G6=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B6)-1))</f>
-        <v/>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="1" t="str">
+        <f>IF(OR(H6="No",H6=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B6)-1))</f>
+        <v/>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="str">
         <f>IF(B7="","",CONCATENATE(Configuration!$A$2,"_",ROW(B7)-1))</f>
         <v>ATP_ProdSpec_6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="1" t="str">
-        <f>IF(OR(G7="No",G7=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B7)-1))</f>
-        <v/>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="str">
+        <f>IF(OR(H7="No",H7=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B7)-1))</f>
+        <v/>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>IF(B8="","",CONCATENATE(Configuration!$A$2,"_",ROW(B8)-1))</f>
         <v>ATP_ProdSpec_7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="str">
-        <f>IF(OR(G8="No",G8=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B8)-1))</f>
-        <v/>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f>IF(OR(H8="No",H8=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B8)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(B9="","",CONCATENATE(Configuration!$A$2,"_",ROW(B9)-1))</f>
         <v>ATP_ProdSpec_8</v>
@@ -850,93 +1150,93 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="str">
-        <f>IF(OR(G9="No",G9=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B9)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f>IF(OR(H9="No",H9=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B9)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f>IF(B10="","",CONCATENATE(Configuration!$A$2,"_",ROW(B10)-1))</f>
         <v>ATP_ProdSpec_9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="str">
-        <f>IF(OR(G10="No",G10=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B10)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f>IF(OR(H10="No",H10=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B10)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="str">
         <f>IF(B11="","",CONCATENATE(Configuration!$A$2,"_",ROW(B11)-1))</f>
         <v>ATP_ProdSpec_10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="str">
-        <f>IF(OR(G11="No",G11=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B11)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3" t="str">
+        <f>IF(OR(H11="No",H11=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B11)-1))</f>
+        <v/>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f>IF(B12="","",CONCATENATE(Configuration!$A$2,"_",ROW(B12)-1))</f>
         <v>ATP_ProdSpec_11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="str">
-        <f>IF(OR(G12="No",G12=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B12)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f>IF(OR(H12="No",H12=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B12)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f>IF(B13="","",CONCATENATE(Configuration!$A$2,"_",ROW(B13)-1))</f>
         <v>ATP_ProdSpec_12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="1" t="str">
-        <f>IF(OR(G13="No",G13=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B13)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="str">
+        <f>IF(OR(H13="No",H13=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B13)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f>IF(B14="","",CONCATENATE(Configuration!$A$2,"_",ROW(B14)-1))</f>
         <v>ATP_ProdSpec_13</v>
@@ -944,33 +1244,34 @@
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="1" t="str">
-        <f>IF(OR(G14="No",G14=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B14)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f>IF(OR(H14="No",H14=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B14)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f>IF(B15="","",CONCATENATE(Configuration!$A$2,"_",ROW(B15)-1))</f>
         <v>ATP_ProdSpec_14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="1" t="str">
-        <f>IF(OR(G15="No",G15=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B15)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f>IF(OR(H15="No",H15=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B15)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f>IF(B16="","",CONCATENATE(Configuration!$A$2,"_",ROW(B16)-1))</f>
         <v>ATP_ProdSpec_15</v>
@@ -978,16 +1279,15 @@
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="1" t="str">
-        <f>IF(OR(G16="No",G16=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B16)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f>IF(OR(H16="No",H16=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B16)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f>IF(B17="","",CONCATENATE(Configuration!$A$2,"_",ROW(B17)-1))</f>
         <v>ATP_ProdSpec_16</v>
@@ -995,33 +1295,31 @@
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="1" t="str">
-        <f>IF(OR(G17="No",G17=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B17)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f>IF(OR(H17="No",H17=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B17)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f>IF(B18="","",CONCATENATE(Configuration!$A$2,"_",ROW(B18)-1))</f>
         <v>ATP_ProdSpec_17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="1" t="str">
-        <f>IF(OR(G18="No",G18=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B18)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f>IF(OR(H18="No",H18=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B18)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f>IF(B19="","",CONCATENATE(Configuration!$A$2,"_",ROW(B19)-1))</f>
         <v>ATP_ProdSpec_18</v>
@@ -1029,33 +1327,31 @@
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="1" t="str">
-        <f>IF(OR(G19="No",G19=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B19)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f>IF(OR(H19="No",H19=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B19)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f>IF(B20="","",CONCATENATE(Configuration!$A$2,"_",ROW(B20)-1))</f>
         <v>ATP_ProdSpec_19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="1" t="str">
-        <f>IF(OR(G20="No",G20=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B20)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f>IF(OR(H20="No",H20=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B20)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f>IF(B21="","",CONCATENATE(Configuration!$A$2,"_",ROW(B21)-1))</f>
         <v>ATP_ProdSpec_20</v>
@@ -1063,16 +1359,15 @@
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="1" t="str">
-        <f>IF(OR(G21="No",G21=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B21)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f>IF(OR(H21="No",H21=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B21)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
         <f>IF(B22="","",CONCATENATE(Configuration!$A$2,"_",ROW(B22)-1))</f>
         <v>ATP_ProdSpec_21</v>
@@ -1080,16 +1375,15 @@
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1" t="str">
-        <f>IF(OR(G22="No",G22=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B22)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f>IF(OR(H22="No",H22=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B22)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
         <f>IF(B23="","",CONCATENATE(Configuration!$A$2,"_",ROW(B23)-1))</f>
         <v>ATP_ProdSpec_22</v>
@@ -1097,16 +1391,15 @@
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1" t="str">
-        <f>IF(OR(G23="No",G23=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B23)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f>IF(OR(H23="No",H23=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B23)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
         <f>IF(B24="","",CONCATENATE(Configuration!$A$2,"_",ROW(B24)-1))</f>
         <v>ATP_ProdSpec_23</v>
@@ -1114,16 +1407,18 @@
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="1" t="str">
-        <f>IF(OR(G24="No",G24=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B24)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <f>IF(OR(H24="No",H24=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B24)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
         <f>IF(B25="","",CONCATENATE(Configuration!$A$2,"_",ROW(B25)-1))</f>
         <v>ATP_ProdSpec_24</v>
@@ -1131,16 +1426,15 @@
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="str">
-        <f>IF(OR(G25="No",G25=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B25)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <f>IF(OR(H25="No",H25=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B25)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="str">
         <f>IF(B26="","",CONCATENATE(Configuration!$A$2,"_",ROW(B26)-1))</f>
         <v>ATP_ProdSpec_25</v>
@@ -1148,16 +1442,15 @@
       <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="1" t="str">
-        <f>IF(OR(G26="No",G26=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B26)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f>IF(OR(H26="No",H26=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B26)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="str">
         <f>IF(B27="","",CONCATENATE(Configuration!$A$2,"_",ROW(B27)-1))</f>
         <v>ATP_ProdSpec_26</v>
@@ -1165,16 +1458,15 @@
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="1" t="str">
-        <f>IF(OR(G27="No",G27=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B27)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <f>IF(OR(H27="No",H27=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B27)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="str">
         <f>IF(B28="","",CONCATENATE(Configuration!$A$2,"_",ROW(B28)-1))</f>
         <v>ATP_ProdSpec_27</v>
@@ -1182,33 +1474,31 @@
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="1" t="str">
-        <f>IF(OR(G28="No",G28=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B28)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <f>IF(OR(H28="No",H28=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B28)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
         <f>IF(B29="","",CONCATENATE(Configuration!$A$2,"_",ROW(B29)-1))</f>
         <v>ATP_ProdSpec_28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="1" t="str">
-        <f>IF(OR(G29="No",G29=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B29)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="1" t="str">
+        <f>IF(OR(H29="No",H29=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B29)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">
         <f>IF(B30="","",CONCATENATE(Configuration!$A$2,"_",ROW(B30)-1))</f>
         <v>ATP_ProdSpec_29</v>
@@ -1216,16 +1506,18 @@
       <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="1" t="str">
-        <f>IF(OR(G30="No",G30=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B30)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <f>IF(OR(H30="No",H30=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B30)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
         <f>IF(B31="","",CONCATENATE(Configuration!$A$2,"_",ROW(B31)-1))</f>
         <v>ATP_ProdSpec_30</v>
@@ -1233,33 +1525,31 @@
       <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="1" t="str">
-        <f>IF(OR(G31="No",G31=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B31)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <f>IF(OR(H31="No",H31=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B31)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
         <f>IF(B32="","",CONCATENATE(Configuration!$A$2,"_",ROW(B32)-1))</f>
         <v>ATP_ProdSpec_31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="1" t="str">
-        <f>IF(OR(G32="No",G32=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B32)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="1" t="str">
+        <f>IF(OR(H32="No",H32=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B32)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
         <f>IF(B33="","",CONCATENATE(Configuration!$A$2,"_",ROW(B33)-1))</f>
         <v>ATP_ProdSpec_32</v>
@@ -1267,16 +1557,18 @@
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="1" t="str">
-        <f>IF(OR(G33="No",G33=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B33)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <f>IF(OR(H33="No",H33=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B33)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
         <f>IF(B34="","",CONCATENATE(Configuration!$A$2,"_",ROW(B34)-1))</f>
         <v>ATP_ProdSpec_33</v>
@@ -1284,289 +1576,662 @@
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="1" t="str">
-        <f>IF(OR(G34="No",G34=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B34)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f>IF(OR(H34="No",H34=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B34)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="str">
         <f>IF(B35="","",CONCATENATE(Configuration!$A$2,"_",ROW(B35)-1))</f>
-        <v/>
+        <v>ATP_ProdSpec_34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f>IF(OR(H35="No",H35=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B35)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="str">
         <f>IF(B36="","",CONCATENATE(Configuration!$A$2,"_",ROW(B36)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f>IF(OR(H36="No",H36=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B36)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="str">
         <f>IF(B37="","",CONCATENATE(Configuration!$A$2,"_",ROW(B37)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f>IF(OR(H37="No",H37=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B37)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="str">
         <f>IF(B38="","",CONCATENATE(Configuration!$A$2,"_",ROW(B38)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f>IF(OR(H38="No",H38=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B38)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="str">
         <f>IF(B39="","",CONCATENATE(Configuration!$A$2,"_",ROW(B39)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f>IF(OR(H39="No",H39=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B39)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="str">
         <f>IF(B40="","",CONCATENATE(Configuration!$A$2,"_",ROW(B40)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="str">
+        <v>ATP_ProdSpec_39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" s="1" t="str">
+        <f>IF(OR(H40="No",H40=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B40)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="str">
         <f>IF(B41="","",CONCATENATE(Configuration!$A$2,"_",ROW(B41)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="3" t="str">
+        <f>IF(OR(H41="No",H41=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B41)-1))</f>
+        <v/>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="str">
         <f>IF(B42="","",CONCATENATE(Configuration!$A$2,"_",ROW(B42)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" s="1" t="str">
+        <f>IF(OR(H42="No",H42=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B42)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="str">
         <f>IF(B43="","",CONCATENATE(Configuration!$A$2,"_",ROW(B43)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="1" t="str">
+        <f>IF(OR(H43="No",H43=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B43)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="str">
         <f>IF(B44="","",CONCATENATE(Configuration!$A$2,"_",ROW(B44)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G44" s="6" t="str">
+        <f>IF(OR(H44="No",H44=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B44)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="str">
         <f>IF(B45="","",CONCATENATE(Configuration!$A$2,"_",ROW(B45)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G45" s="6" t="str">
+        <f>IF(OR(H45="No",H45=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B45)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="str">
         <f>IF(B46="","",CONCATENATE(Configuration!$A$2,"_",ROW(B46)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G46" s="1" t="str">
+        <f>IF(OR(H46="No",H46=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B46)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="str">
         <f>IF(B47="","",CONCATENATE(Configuration!$A$2,"_",ROW(B47)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G47" s="1" t="str">
+        <f>IF(OR(H47="No",H47=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B47)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="str">
         <f>IF(B48="","",CONCATENATE(Configuration!$A$2,"_",ROW(B48)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G48" s="1" t="str">
+        <f>IF(OR(H48="No",H48=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B48)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="str">
         <f>IF(B49="","",CONCATENATE(Configuration!$A$2,"_",ROW(B49)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" s="1" t="str">
+        <f>IF(OR(H49="No",H49=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B49)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="str">
         <f>IF(B50="","",CONCATENATE(Configuration!$A$2,"_",ROW(B50)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G50" s="1" t="str">
+        <f>IF(OR(H50="No",H50=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B50)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="str">
         <f>IF(B51="","",CONCATENATE(Configuration!$A$2,"_",ROW(B51)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G51" s="1" t="str">
+        <f>IF(OR(H51="No",H51=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B51)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="str">
         <f>IF(B52="","",CONCATENATE(Configuration!$A$2,"_",ROW(B52)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G52" s="6" t="str">
+        <f>IF(OR(H52="No",H52=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B52)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="str">
         <f>IF(B53="","",CONCATENATE(Configuration!$A$2,"_",ROW(B53)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="6" t="str">
+        <f>IF(OR(H53="No",H53=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B53)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="str">
         <f>IF(B54="","",CONCATENATE(Configuration!$A$2,"_",ROW(B54)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" s="6" t="str">
+        <f>IF(OR(H54="No",H54=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B54)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="str">
         <f>IF(B55="","",CONCATENATE(Configuration!$A$2,"_",ROW(B55)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G55" s="6" t="str">
+        <f>IF(OR(H55="No",H55=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B55)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="str">
         <f>IF(B56="","",CONCATENATE(Configuration!$A$2,"_",ROW(B56)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G56" s="1" t="str">
+        <f>IF(OR(H56="No",H56=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B56)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="str">
         <f>IF(B57="","",CONCATENATE(Configuration!$A$2,"_",ROW(B57)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="1" t="str">
+        <f>IF(OR(H57="No",H57=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B57)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="str">
         <f>IF(B58="","",CONCATENATE(Configuration!$A$2,"_",ROW(B58)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G58" s="1" t="str">
+        <f>IF(OR(H58="No",H58=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B58)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="str">
         <f>IF(B59="","",CONCATENATE(Configuration!$A$2,"_",ROW(B59)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="str">
+        <v>ATP_ProdSpec_58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G59" s="1" t="str">
+        <f>IF(OR(H59="No",H59=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B59)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="str">
         <f>IF(B60="","",CONCATENATE(Configuration!$A$2,"_",ROW(B60)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" s="3" t="str">
+        <f>IF(OR(H60="No",H60=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B60)-1))</f>
+        <v/>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="str">
         <f>IF(B61="","",CONCATENATE(Configuration!$A$2,"_",ROW(B61)-1))</f>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C61" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G61" s="1" t="str">
+        <f>IF(OR(H61="No",H61=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B61)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="str">
         <f>IF(B62="","",CONCATENATE(Configuration!$A$2,"_",ROW(B62)-1))</f>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G62" s="1" t="str">
+        <f>IF(OR(H62="No",H62=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B62)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="str">
         <f>IF(B63="","",CONCATENATE(Configuration!$A$2,"_",ROW(B63)-1))</f>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C63" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G63" s="1" t="str">
+        <f>IF(OR(H63="No",H63=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B63)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="str">
         <f>IF(B64="","",CONCATENATE(Configuration!$A$2,"_",ROW(B64)-1))</f>
         <v/>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="str">
+      <c r="C64" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G64" s="1" t="str">
+        <f>IF(OR(H64="No",H64=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B64)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="str">
         <f>IF(B65="","",CONCATENATE(Configuration!$A$2,"_",ROW(B65)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="str">
+        <v>ATP_ProdSpec_64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65" s="3" t="str">
+        <f>IF(OR(H65="No",H65=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B65)-1))</f>
+        <v/>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="str">
         <f>IF(B66="","",CONCATENATE(Configuration!$A$2,"_",ROW(B66)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_65</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="3" t="str">
+        <f>IF(OR(H66="No",H66=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B66)-1))</f>
+        <v/>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="str">
         <f>IF(B67="","",CONCATENATE(Configuration!$A$2,"_",ROW(B67)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="1" t="str">
+        <f>IF(OR(H67="No",H67=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B67)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="str">
         <f>IF(B68="","",CONCATENATE(Configuration!$A$2,"_",ROW(B68)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="1" t="str">
+        <f>IF(OR(H68="No",H68=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B68)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="str">
         <f>IF(B69="","",CONCATENATE(Configuration!$A$2,"_",ROW(B69)-1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+        <v>ATP_ProdSpec_68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" s="1" t="str">
+        <f>IF(OR(H69="No",H69=""),"",CONCATENATE(Configuration!$A$2,"_TC_",ROW(B69)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="str">
         <f>IF(B70="","",CONCATENATE(Configuration!$A$2,"_",ROW(B70)-1))</f>
         <v/>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C70" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="str">
         <f>IF(B71="","",CONCATENATE(Configuration!$A$2,"_",ROW(B71)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="str">
         <f>IF(B72="","",CONCATENATE(Configuration!$A$2,"_",ROW(B72)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="str">
         <f>IF(B73="","",CONCATENATE(Configuration!$A$2,"_",ROW(B73)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="str">
         <f>IF(B74="","",CONCATENATE(Configuration!$A$2,"_",ROW(B74)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="str">
         <f>IF(B75="","",CONCATENATE(Configuration!$A$2,"_",ROW(B75)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="str">
         <f>IF(B76="","",CONCATENATE(Configuration!$A$2,"_",ROW(B76)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="str">
         <f>IF(B77="","",CONCATENATE(Configuration!$A$2,"_",ROW(B77)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="str">
         <f>IF(B78="","",CONCATENATE(Configuration!$A$2,"_",ROW(B78)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="str">
         <f>IF(B79="","",CONCATENATE(Configuration!$A$2,"_",ROW(B79)-1))</f>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="str">
         <f>IF(B80="","",CONCATENATE(Configuration!$A$2,"_",ROW(B80)-1))</f>
         <v/>
@@ -4137,6 +4802,216 @@
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" s="1" t="str">
         <f>IF(B508="","",CONCATENATE(Configuration!$A$2,"_",ROW(B508)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="1" t="str">
+        <f>IF(B509="","",CONCATENATE(Configuration!$A$2,"_",ROW(B509)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="1" t="str">
+        <f>IF(B510="","",CONCATENATE(Configuration!$A$2,"_",ROW(B510)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="1" t="str">
+        <f>IF(B511="","",CONCATENATE(Configuration!$A$2,"_",ROW(B511)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="1" t="str">
+        <f>IF(B512="","",CONCATENATE(Configuration!$A$2,"_",ROW(B512)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="1" t="str">
+        <f>IF(B513="","",CONCATENATE(Configuration!$A$2,"_",ROW(B513)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="1" t="str">
+        <f>IF(B514="","",CONCATENATE(Configuration!$A$2,"_",ROW(B514)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="1" t="str">
+        <f>IF(B515="","",CONCATENATE(Configuration!$A$2,"_",ROW(B515)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="1" t="str">
+        <f>IF(B516="","",CONCATENATE(Configuration!$A$2,"_",ROW(B516)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="1" t="str">
+        <f>IF(B517="","",CONCATENATE(Configuration!$A$2,"_",ROW(B517)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="1" t="str">
+        <f>IF(B518="","",CONCATENATE(Configuration!$A$2,"_",ROW(B518)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="1" t="str">
+        <f>IF(B519="","",CONCATENATE(Configuration!$A$2,"_",ROW(B519)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="1" t="str">
+        <f>IF(B520="","",CONCATENATE(Configuration!$A$2,"_",ROW(B520)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="1" t="str">
+        <f>IF(B521="","",CONCATENATE(Configuration!$A$2,"_",ROW(B521)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="1" t="str">
+        <f>IF(B522="","",CONCATENATE(Configuration!$A$2,"_",ROW(B522)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="1" t="str">
+        <f>IF(B523="","",CONCATENATE(Configuration!$A$2,"_",ROW(B523)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="1" t="str">
+        <f>IF(B524="","",CONCATENATE(Configuration!$A$2,"_",ROW(B524)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="1" t="str">
+        <f>IF(B525="","",CONCATENATE(Configuration!$A$2,"_",ROW(B525)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="1" t="str">
+        <f>IF(B526="","",CONCATENATE(Configuration!$A$2,"_",ROW(B526)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="1" t="str">
+        <f>IF(B527="","",CONCATENATE(Configuration!$A$2,"_",ROW(B527)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" s="1" t="str">
+        <f>IF(B528="","",CONCATENATE(Configuration!$A$2,"_",ROW(B528)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" s="1" t="str">
+        <f>IF(B529="","",CONCATENATE(Configuration!$A$2,"_",ROW(B529)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" s="1" t="str">
+        <f>IF(B530="","",CONCATENATE(Configuration!$A$2,"_",ROW(B530)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" s="1" t="str">
+        <f>IF(B531="","",CONCATENATE(Configuration!$A$2,"_",ROW(B531)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" s="1" t="str">
+        <f>IF(B532="","",CONCATENATE(Configuration!$A$2,"_",ROW(B532)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" s="1" t="str">
+        <f>IF(B533="","",CONCATENATE(Configuration!$A$2,"_",ROW(B533)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" s="1" t="str">
+        <f>IF(B534="","",CONCATENATE(Configuration!$A$2,"_",ROW(B534)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" s="1" t="str">
+        <f>IF(B535="","",CONCATENATE(Configuration!$A$2,"_",ROW(B535)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" s="1" t="str">
+        <f>IF(B536="","",CONCATENATE(Configuration!$A$2,"_",ROW(B536)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" s="1" t="str">
+        <f>IF(B537="","",CONCATENATE(Configuration!$A$2,"_",ROW(B537)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" s="1" t="str">
+        <f>IF(B538="","",CONCATENATE(Configuration!$A$2,"_",ROW(B538)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" s="1" t="str">
+        <f>IF(B539="","",CONCATENATE(Configuration!$A$2,"_",ROW(B539)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" s="1" t="str">
+        <f>IF(B540="","",CONCATENATE(Configuration!$A$2,"_",ROW(B540)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" s="1" t="str">
+        <f>IF(B541="","",CONCATENATE(Configuration!$A$2,"_",ROW(B541)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" s="1" t="str">
+        <f>IF(B542="","",CONCATENATE(Configuration!$A$2,"_",ROW(B542)-1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" s="1" t="str">
+        <f>IF(B543="","",CONCATENATE(Configuration!$A$2,"_",ROW(B543)-1))</f>
         <v/>
       </c>
     </row>
@@ -4150,30 +5025,36 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{36EFAC8E-5F6E-4CD9-A68D-9CC1EA23F2A7}">
-          <x14:formula1>
-            <xm:f>Configuration!$C$2:$C$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D34</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF58A4B9-216D-4E27-BC79-3A26FE068C30}">
           <x14:formula1>
             <xm:f>Configuration!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I34</xm:sqref>
+          <xm:sqref>J2:J69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C384262D-E1BB-4157-9D06-D62A59903D66}">
           <x14:formula1>
             <xm:f>Configuration!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G34</xm:sqref>
+          <xm:sqref>H2:H69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{36EFAC8E-5F6E-4CD9-A68D-9CC1EA23F2A7}">
+          <x14:formula1>
+            <xm:f>Configuration!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:E69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{81F71362-FB71-45F6-9FCF-7C3A39DC8545}">
           <x14:formula1>
             <xm:f>Configuration!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B35</xm:sqref>
+          <xm:sqref>B2:B70</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33F73015-4FD4-49A1-908A-9E37DCB94926}">
+          <x14:formula1>
+            <xm:f>Configuration!$F$2:$F$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F70</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4183,10 +5064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615C6A32-B606-4753-AC4E-A09D86FFD84B}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4196,9 +5077,10 @@
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -4214,13 +5096,16 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -4231,8 +5116,11 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -4245,8 +5133,11 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -4260,7 +5151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -4271,7 +5162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -4282,19 +5173,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>